<commit_message>
Planning Documents & Data Model
</commit_message>
<xml_diff>
--- a/Data/DataDictionary.xlsx
+++ b/Data/DataDictionary.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/286e2ff89c220aa4/Documents/University of Rochester/M2/DSCC483_DataScienceCapstone/URMCVenitaltorAllocation/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_F25DC773A252ABDACC1048AE991E56DC5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4F4599B-552E-4507-BE5C-A0CFA18900EE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DataDictionary" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,15 +24,182 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
+  <si>
+    <t>Dataset Name</t>
+  </si>
+  <si>
+    <t>Data field name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Study_Cohort_DeID</t>
+  </si>
+  <si>
+    <t>seq</t>
+  </si>
+  <si>
+    <t>Encounter_Number</t>
+  </si>
+  <si>
+    <t>SubjectID</t>
+  </si>
+  <si>
+    <t>Subject ID</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Ethnicity</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Discharge_Status</t>
+  </si>
+  <si>
+    <t>Length_of_Stay (days)</t>
+  </si>
+  <si>
+    <t>Age_at_Admission</t>
+  </si>
+  <si>
+    <t>Admission_dXs_DeID</t>
+  </si>
+  <si>
+    <t>ICD10_dX(s)</t>
+  </si>
+  <si>
+    <t>ICD-10-CM code of admission diagnosis</t>
+  </si>
+  <si>
+    <t>dX_Name</t>
+  </si>
+  <si>
+    <t>Reason_Visit</t>
+  </si>
+  <si>
+    <t>Insurance_DeID</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Name of insurance payer</t>
+  </si>
+  <si>
+    <t>BLIS_Assessment_DeID</t>
+  </si>
+  <si>
+    <t>seq_num</t>
+  </si>
+  <si>
+    <t>intubation_number</t>
+  </si>
+  <si>
+    <t>assessment_timepoint</t>
+  </si>
+  <si>
+    <t>vent_duration (hours)</t>
+  </si>
+  <si>
+    <t>sofa_score</t>
+  </si>
+  <si>
+    <t>SOFA score</t>
+  </si>
+  <si>
+    <t>assessment_color</t>
+  </si>
+  <si>
+    <t>COVID Status_DeID</t>
+  </si>
+  <si>
+    <t>covid_positive_lab</t>
+  </si>
+  <si>
+    <t>covid_positive_strong_dx</t>
+  </si>
+  <si>
+    <t>covid_positive_weak_dx</t>
+  </si>
+  <si>
+    <t>COVID_POSITIVE_N3C_Phenotype</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>De-identified numeric hospital admission encounter sequence number</t>
+  </si>
+  <si>
+    <t>Discharge status of hospital stay</t>
+  </si>
+  <si>
+    <t>Length of hospital stay in days</t>
+  </si>
+  <si>
+    <t>Subject's age at hospital admission. The value is masked with &gt;90 when subject is 90 years old or older at the time of hospital admission</t>
+  </si>
+  <si>
+    <t>Name of diagnsis</t>
+  </si>
+  <si>
+    <t>Reason for visit</t>
+  </si>
+  <si>
+    <t>ID or Links to EncounterID?</t>
+  </si>
+  <si>
+    <t>Sequence number of intubation(s) each subject has</t>
+  </si>
+  <si>
+    <t>Numeric assessment timepoint by VAP (initial assesment = 0, thereafter starting at 5, 6, 7 etc.)</t>
+  </si>
+  <si>
+    <t>Length of ventilator use in hours</t>
+  </si>
+  <si>
+    <t>Color code assigned at assessment</t>
+  </si>
+  <si>
+    <t>Indicator if subject meets the N3C COVID positive rule with eligible laboratory evidence</t>
+  </si>
+  <si>
+    <t>Indicator if subject meets the N3C COVID positive rule with eligible diagnoses of strong diagose codes</t>
+  </si>
+  <si>
+    <t>Indicator if subject meets the N3C COVID positive rule with eligible diagnoses of weak diagose codes</t>
+  </si>
+  <si>
+    <t>Indicator if subject meets the phenotype rules (*) N3C COVID positive( such that if any "yes" for  Covid_lab, strong_dx or weak_dx, then covid_positive_n3c_phenotype is yes)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,13 +222,105 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +331,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7AE6F18A-F77E-49EA-B20E-BFBFAD65A1C7}" name="DataDictionary" displayName="DataDictionary" ref="A1:C33" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:C33" xr:uid="{7AE6F18A-F77E-49EA-B20E-BFBFAD65A1C7}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8005ED2D-3F78-47DD-AA7E-653CA6A27594}" name="Dataset Name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{17EA66AC-3729-41F1-8E1C-067228274F4A}" name="Data field name" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{CE1DDE9E-F902-4E85-800F-40C671DFBD0C}" name="Description" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +607,386 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="159.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>